<commit_message>
Added multiple orders to the same address and minor bug fixes
</commit_message>
<xml_diff>
--- a/SKU.xlsx
+++ b/SKU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rapolas_PC\PycharmProjects\ExcelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD89782-53B5-41D1-81D4-DD86EC477E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FCC8D6-43E3-4B21-BE5C-06DA3CA54178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>SKU</t>
   </si>
@@ -235,6 +235,102 @@
   </si>
   <si>
     <t>KEP</t>
+  </si>
+  <si>
+    <t>MBV L</t>
+  </si>
+  <si>
+    <t>MBK XL</t>
+  </si>
+  <si>
+    <t>SW M</t>
+  </si>
+  <si>
+    <t>MBK L</t>
+  </si>
+  <si>
+    <t>MBK M</t>
+  </si>
+  <si>
+    <t>MBK S</t>
+  </si>
+  <si>
+    <t>MBV M</t>
+  </si>
+  <si>
+    <t>MBV XL</t>
+  </si>
+  <si>
+    <t>MBV S</t>
+  </si>
+  <si>
+    <t>HO M</t>
+  </si>
+  <si>
+    <t>HO XL</t>
+  </si>
+  <si>
+    <t>HO L</t>
+  </si>
+  <si>
+    <t>HO S</t>
+  </si>
+  <si>
+    <t>SW XL</t>
+  </si>
+  <si>
+    <t>SW L</t>
+  </si>
+  <si>
+    <t>SW S</t>
+  </si>
+  <si>
+    <t>MPM L</t>
+  </si>
+  <si>
+    <t>MPM XL</t>
+  </si>
+  <si>
+    <t>MPM M</t>
+  </si>
+  <si>
+    <t>MPM S</t>
+  </si>
+  <si>
+    <t>MBM S</t>
+  </si>
+  <si>
+    <t>MBM XL</t>
+  </si>
+  <si>
+    <t>MBM L</t>
+  </si>
+  <si>
+    <t>MBM M</t>
+  </si>
+  <si>
+    <t>MPV XL</t>
+  </si>
+  <si>
+    <t>MPV L</t>
+  </si>
+  <si>
+    <t>MPV M</t>
+  </si>
+  <si>
+    <t>MPV S</t>
+  </si>
+  <si>
+    <t>MBK XXL</t>
+  </si>
+  <si>
+    <t>MPV XXL</t>
+  </si>
+  <si>
+    <t>MPV XS</t>
+  </si>
+  <si>
+    <t>MBK XS</t>
   </si>
 </sst>
 </file>
@@ -552,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70:G71"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,6 +1404,358 @@
         <v>13</v>
       </c>
     </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69">
+        <v>115</v>
+      </c>
+      <c r="C69">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>115</v>
+      </c>
+      <c r="C70">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71">
+        <v>127</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72">
+        <v>137</v>
+      </c>
+      <c r="C72">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73">
+        <v>145</v>
+      </c>
+      <c r="C73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74">
+        <v>145</v>
+      </c>
+      <c r="C74">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75">
+        <v>160</v>
+      </c>
+      <c r="C75">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76">
+        <v>115</v>
+      </c>
+      <c r="C76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>127</v>
+      </c>
+      <c r="C77">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>137</v>
+      </c>
+      <c r="C78">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79">
+        <v>145</v>
+      </c>
+      <c r="C79">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80">
+        <v>160</v>
+      </c>
+      <c r="C80">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>125</v>
+      </c>
+      <c r="C81">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>129</v>
+      </c>
+      <c r="C82">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <v>115</v>
+      </c>
+      <c r="C83">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>127</v>
+      </c>
+      <c r="C84">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85">
+        <v>137</v>
+      </c>
+      <c r="C85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>145</v>
+      </c>
+      <c r="C86">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>160</v>
+      </c>
+      <c r="C87">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>115</v>
+      </c>
+      <c r="C88">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>127</v>
+      </c>
+      <c r="C89">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>137</v>
+      </c>
+      <c r="C90">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>145</v>
+      </c>
+      <c r="C91">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92">
+        <v>160</v>
+      </c>
+      <c r="C92">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93">
+        <v>115</v>
+      </c>
+      <c r="C93">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94">
+        <v>127</v>
+      </c>
+      <c r="C94">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95">
+        <v>160</v>
+      </c>
+      <c r="C95">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>160</v>
+      </c>
+      <c r="C96">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>115</v>
+      </c>
+      <c r="C97">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>160</v>
+      </c>
+      <c r="C98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>115</v>
+      </c>
+      <c r="C99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>115</v>
+      </c>
+      <c r="C100">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>